<commit_message>
Added figure, saved svgs
</commit_message>
<xml_diff>
--- a/Accuracies and confusion matrices (from part 4 script).xlsx
+++ b/Accuracies and confusion matrices (from part 4 script).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rdman\Desktop\Open-Data-MeadoWatch_2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A05A7577-CB92-4407-8480-ED8A0A31458A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A2487E1-A728-4B16-93EC-D73F0F57050E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="2" xr2:uid="{7387BE08-8C25-4F12-B722-D4BDEBCED174}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="23040" windowHeight="12204" xr2:uid="{7387BE08-8C25-4F12-B722-D4BDEBCED174}"/>
   </bookViews>
   <sheets>
     <sheet name="Confusion mat trails sp" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="41">
   <si>
     <t>scientists</t>
   </si>
@@ -152,12 +152,21 @@
   </si>
   <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>PERC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="169" formatCode="0.000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -187,8 +196,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -503,25 +513,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{751CF589-9227-46A2-9D88-64A163A95440}">
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="6" max="7" width="10.5546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C3" t="s">
         <v>2</v>
       </c>
@@ -529,7 +545,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -542,8 +558,23 @@
       <c r="D4">
         <v>180</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F4" s="1">
+        <f>C4/$J$4</f>
+        <v>0.25394190871369293</v>
+      </c>
+      <c r="G4" s="1">
+        <f>D4/$J$4</f>
+        <v>7.4688796680497924E-2</v>
+      </c>
+      <c r="I4" t="s">
+        <v>39</v>
+      </c>
+      <c r="J4">
+        <f>C4+D4+C5+D5</f>
+        <v>2410</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>3</v>
       </c>
@@ -553,16 +584,26 @@
       <c r="D5">
         <v>1376</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F5" s="1">
+        <f>C5/$J$4</f>
+        <v>0.1004149377593361</v>
+      </c>
+      <c r="G5" s="1">
+        <f>D5/$J$4</f>
+        <v>0.570954356846473</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
         <v>4</v>
       </c>
       <c r="D6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>4</v>
       </c>
@@ -572,8 +613,23 @@
       <c r="D7">
         <v>108</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F7" s="1">
+        <f>C7/$J$7</f>
+        <v>0.2391304347826087</v>
+      </c>
+      <c r="G7" s="1">
+        <f>D7/$J$7</f>
+        <v>4.51505016722408E-2</v>
+      </c>
+      <c r="I7" t="s">
+        <v>39</v>
+      </c>
+      <c r="J7">
+        <f t="shared" ref="J5:J30" si="0">C7+D7+C8+D8</f>
+        <v>2392</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>5</v>
       </c>
@@ -583,16 +639,26 @@
       <c r="D8">
         <v>1565</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F8" s="1">
+        <f t="shared" ref="F8:F9" si="1">C8/$J$7</f>
+        <v>6.145484949832776E-2</v>
+      </c>
+      <c r="G8" s="1">
+        <f t="shared" ref="G8:G9" si="2">D8/$J$7</f>
+        <v>0.65426421404682278</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
         <v>6</v>
       </c>
       <c r="D9" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>6</v>
       </c>
@@ -602,8 +668,23 @@
       <c r="D10">
         <v>143</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F10" s="1">
+        <f>C10/$J$10</f>
+        <v>0.12111017661900757</v>
+      </c>
+      <c r="G10" s="1">
+        <f>D10/$J$10</f>
+        <v>6.0134566862910008E-2</v>
+      </c>
+      <c r="I10" t="s">
+        <v>39</v>
+      </c>
+      <c r="J10">
+        <f>C10+D10+C11+D11</f>
+        <v>2378</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>7</v>
       </c>
@@ -613,16 +694,26 @@
       <c r="D11">
         <v>1818</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F11" s="1">
+        <f>C11/$J$10</f>
+        <v>5.4247266610597138E-2</v>
+      </c>
+      <c r="G11" s="1">
+        <f>D11/$J$10</f>
+        <v>0.76450798990748525</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C12" t="s">
         <v>8</v>
       </c>
       <c r="D12" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>8</v>
       </c>
@@ -632,8 +723,23 @@
       <c r="D13">
         <v>84</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F13" s="1">
+        <f>C13/$J$13</f>
+        <v>2.9150823827629912E-2</v>
+      </c>
+      <c r="G13" s="1">
+        <f>D13/$J$13</f>
+        <v>3.5487959442332066E-2</v>
+      </c>
+      <c r="I13" t="s">
+        <v>39</v>
+      </c>
+      <c r="J13">
+        <f>C13+D13+C14+D14</f>
+        <v>2367</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>9</v>
       </c>
@@ -643,26 +749,46 @@
       <c r="D14">
         <v>2132</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F14" s="1">
+        <f>C14/$J$13</f>
+        <v>3.4643008027038444E-2</v>
+      </c>
+      <c r="G14" s="1">
+        <f>D14/$J$13</f>
+        <v>0.90071820870299957</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C17" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F17" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C18" t="s">
         <v>2</v>
       </c>
       <c r="D18" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>0</v>
       </c>
@@ -675,8 +801,23 @@
       <c r="D19">
         <v>174</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F19" s="1">
+        <f>C19/$J$19</f>
+        <v>0.15499837186584176</v>
+      </c>
+      <c r="G19" s="1">
+        <f>D19/$J$19</f>
+        <v>5.6659068707261478E-2</v>
+      </c>
+      <c r="I19" t="s">
+        <v>39</v>
+      </c>
+      <c r="J19">
+        <f>C19+D19+C20+D20</f>
+        <v>3071</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>3</v>
       </c>
@@ -686,16 +827,26 @@
       <c r="D20">
         <v>2207</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F20" s="1">
+        <f>C20/$J$19</f>
+        <v>6.9684141973298599E-2</v>
+      </c>
+      <c r="G20" s="1">
+        <f>D20/$J$19</f>
+        <v>0.71865841745359815</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C21" t="s">
         <v>4</v>
       </c>
       <c r="D21" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>4</v>
       </c>
@@ -705,8 +856,23 @@
       <c r="D22">
         <v>134</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F22" s="1">
+        <f>C22/$J$22</f>
+        <v>0.16886979510905487</v>
+      </c>
+      <c r="G22" s="1">
+        <f>D22/$J$22</f>
+        <v>4.4282881692002646E-2</v>
+      </c>
+      <c r="I22" t="s">
+        <v>39</v>
+      </c>
+      <c r="J22">
+        <f>C22+D22+C23+D23</f>
+        <v>3026</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>5</v>
       </c>
@@ -716,16 +882,26 @@
       <c r="D23">
         <v>2209</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F23" s="1">
+        <f>C23/$J$22</f>
+        <v>5.6840713813615336E-2</v>
+      </c>
+      <c r="G23" s="1">
+        <f>D23/$J$22</f>
+        <v>0.73000660938532713</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C24" t="s">
         <v>6</v>
       </c>
       <c r="D24" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>6</v>
       </c>
@@ -735,8 +911,23 @@
       <c r="D25">
         <v>177</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F25" s="1">
+        <f>C25/$J$25</f>
+        <v>0.18000664231152441</v>
+      </c>
+      <c r="G25" s="1">
+        <f>D25/$J$25</f>
+        <v>5.878445699103288E-2</v>
+      </c>
+      <c r="I25" t="s">
+        <v>39</v>
+      </c>
+      <c r="J25">
+        <f>C25+D25+C26+D26</f>
+        <v>3011</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>7</v>
       </c>
@@ -746,16 +937,26 @@
       <c r="D26">
         <v>2110</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F26" s="1">
+        <f>C26/$J$25</f>
+        <v>6.0445034872135504E-2</v>
+      </c>
+      <c r="G26" s="1">
+        <f>D26/$J$25</f>
+        <v>0.70076386582530725</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C27" t="s">
         <v>8</v>
       </c>
       <c r="D27" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>8</v>
       </c>
@@ -765,8 +966,23 @@
       <c r="D28">
         <v>110</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F28" s="1">
+        <f>C28/$J$28</f>
+        <v>8.3499667332002661E-2</v>
+      </c>
+      <c r="G28" s="1">
+        <f>D28/$J$28</f>
+        <v>3.6593479707252165E-2</v>
+      </c>
+      <c r="I28" t="s">
+        <v>39</v>
+      </c>
+      <c r="J28">
+        <f>C28+D28+C29+D29</f>
+        <v>3006</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>9</v>
       </c>
@@ -775,6 +991,14 @@
       </c>
       <c r="D29">
         <v>2462</v>
+      </c>
+      <c r="F29" s="1">
+        <f>C29/$J$28</f>
+        <v>6.0878243512974051E-2</v>
+      </c>
+      <c r="G29" s="1">
+        <f>D29/$J$28</f>
+        <v>0.81902860944777112</v>
       </c>
     </row>
   </sheetData>
@@ -886,7 +1110,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I17:K56">
+  <conditionalFormatting sqref="I31:K56 K17:K30">
     <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min"/>
@@ -1052,7 +1276,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FB27E6F-71FF-48D3-8F9D-CB30443357E8}">
   <dimension ref="A1:H73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>

</xml_diff>